<commit_message>
Added trends for searches
</commit_message>
<xml_diff>
--- a/docs/tinytape redis keys.xlsx
+++ b/docs/tinytape redis keys.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="204">
   <si>
     <t>tinytape_scores</t>
   </si>
@@ -613,6 +613,21 @@
   </si>
   <si>
     <t>Usage data by day</t>
+  </si>
+  <si>
+    <t>tinytape_&lt;time code&gt;_searches</t>
+  </si>
+  <si>
+    <t>Search trends</t>
+  </si>
+  <si>
+    <t>search cound</t>
+  </si>
+  <si>
+    <t>tinytape_&lt;time code&gt;_searches_&lt;username&gt;</t>
+  </si>
+  <si>
+    <t>Search trends by user</t>
   </si>
 </sst>
 </file>
@@ -960,10 +975,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E77" sqref="E77"/>
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2174,6 +2189,40 @@
       </c>
       <c r="E76" t="s">
         <v>198</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>199</v>
+      </c>
+      <c r="B77" t="s">
+        <v>23</v>
+      </c>
+      <c r="C77" t="s">
+        <v>83</v>
+      </c>
+      <c r="D77" t="s">
+        <v>77</v>
+      </c>
+      <c r="E77" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>202</v>
+      </c>
+      <c r="B78" t="s">
+        <v>23</v>
+      </c>
+      <c r="C78" t="s">
+        <v>201</v>
+      </c>
+      <c r="D78" t="s">
+        <v>77</v>
+      </c>
+      <c r="E78" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>